<commit_message>
add Sideroca and Alternative operators
</commit_message>
<xml_diff>
--- a/WriteData/operators.xlsx
+++ b/WriteData/operators.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Web\ArknightsTools\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Web\ArknightsTools\WriteData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE6CEF7-A0C9-42A7-8130-3DDB87DC79CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F5158F-88F1-4DAC-B023-BAFBB8FFBEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="463">
   <si>
     <t>codeName</t>
   </si>
@@ -1385,6 +1385,30 @@
   </si>
   <si>
     <t>Gnosis</t>
+  </si>
+  <si>
+    <t>alter</t>
+  </si>
+  <si>
+    <t>Sideroca</t>
+  </si>
+  <si>
+    <t>Lava the Purgatory</t>
+  </si>
+  <si>
+    <t>Originium crystals distributed across surface of her body, confirmed Infected by medical examination</t>
+  </si>
+  <si>
+    <t>Skadi the Corrupting Heart</t>
+  </si>
+  <si>
+    <t>Medical tests have confirmed that no infection is present. The following discussion summaries are all based upon observations and calculations of the person in question's cell proliferation status</t>
+  </si>
+  <si>
+    <t>Ch'en the Holungday</t>
+  </si>
+  <si>
+    <t>Nearl the Radiant Knight</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1416,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mmm\ d"/>
+    <numFmt numFmtId="164" formatCode="mmm\ d"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1873,7 +1897,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2229,29 +2253,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L212"/>
+  <dimension ref="A1:M217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="E188" sqref="E188"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D219" sqref="D219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="154.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="161.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2288,8 +2314,11 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2326,8 +2355,11 @@
       <c r="L2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2364,8 +2396,11 @@
       <c r="L3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2402,8 +2437,11 @@
       <c r="L4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -2440,8 +2478,11 @@
       <c r="L5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -2478,8 +2519,11 @@
       <c r="L6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -2516,8 +2560,11 @@
       <c r="L7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -2554,8 +2601,11 @@
       <c r="L8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -2592,8 +2642,11 @@
       <c r="L9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -2630,8 +2683,11 @@
       <c r="L10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2668,8 +2724,11 @@
       <c r="L11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -2706,8 +2765,11 @@
       <c r="L12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -2744,8 +2806,11 @@
       <c r="L13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -2782,8 +2847,11 @@
       <c r="L14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -2820,8 +2888,11 @@
       <c r="L15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -2858,8 +2929,11 @@
       <c r="L16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -2896,8 +2970,11 @@
       <c r="L17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -2934,8 +3011,11 @@
       <c r="L18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -2972,8 +3052,11 @@
       <c r="L19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -3010,8 +3093,11 @@
       <c r="L20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -3048,8 +3134,11 @@
       <c r="L21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -3086,8 +3175,11 @@
       <c r="L22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -3124,8 +3216,11 @@
       <c r="L23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -3162,8 +3257,11 @@
       <c r="L24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -3200,8 +3298,11 @@
       <c r="L25" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -3238,8 +3339,11 @@
       <c r="L26" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>101</v>
       </c>
@@ -3276,8 +3380,11 @@
       <c r="L27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -3314,8 +3421,11 @@
       <c r="L28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>107</v>
       </c>
@@ -3352,8 +3462,11 @@
       <c r="L29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -3390,8 +3503,11 @@
       <c r="L30" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>112</v>
       </c>
@@ -3428,8 +3544,11 @@
       <c r="L31" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>113</v>
       </c>
@@ -3466,8 +3585,11 @@
       <c r="L32" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -3504,8 +3626,11 @@
       <c r="L33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>120</v>
       </c>
@@ -3542,8 +3667,11 @@
       <c r="L34" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>122</v>
       </c>
@@ -3580,8 +3708,11 @@
       <c r="L35" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>127</v>
       </c>
@@ -3618,8 +3749,11 @@
       <c r="L36" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -3656,8 +3790,11 @@
       <c r="L37" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -3694,8 +3831,11 @@
       <c r="L38" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -3732,8 +3872,11 @@
       <c r="L39" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -3770,8 +3913,11 @@
       <c r="L40" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>138</v>
       </c>
@@ -3808,8 +3954,11 @@
       <c r="L41" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>141</v>
       </c>
@@ -3846,8 +3995,11 @@
       <c r="L42" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>145</v>
       </c>
@@ -3884,8 +4036,11 @@
       <c r="L43" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>147</v>
       </c>
@@ -3922,8 +4077,11 @@
       <c r="L44" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>150</v>
       </c>
@@ -3960,8 +4118,11 @@
       <c r="L45" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>153</v>
       </c>
@@ -3998,8 +4159,11 @@
       <c r="L46" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>155</v>
       </c>
@@ -4036,8 +4200,11 @@
       <c r="L47" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>157</v>
       </c>
@@ -4074,8 +4241,11 @@
       <c r="L48" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>159</v>
       </c>
@@ -4112,8 +4282,11 @@
       <c r="L49" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>160</v>
       </c>
@@ -4150,8 +4323,11 @@
       <c r="L50" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>164</v>
       </c>
@@ -4188,8 +4364,11 @@
       <c r="L51" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>167</v>
       </c>
@@ -4226,8 +4405,11 @@
       <c r="L52" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -4264,8 +4446,11 @@
       <c r="L53" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>173</v>
       </c>
@@ -4302,8 +4487,11 @@
       <c r="L54" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>174</v>
       </c>
@@ -4340,8 +4528,11 @@
       <c r="L55" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>175</v>
       </c>
@@ -4378,8 +4569,11 @@
       <c r="L56" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>177</v>
       </c>
@@ -4416,8 +4610,11 @@
       <c r="L57" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>178</v>
       </c>
@@ -4454,8 +4651,11 @@
       <c r="L58" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>179</v>
       </c>
@@ -4492,8 +4692,11 @@
       <c r="L59" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>182</v>
       </c>
@@ -4530,8 +4733,11 @@
       <c r="L60" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>184</v>
       </c>
@@ -4568,8 +4774,11 @@
       <c r="L61" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>186</v>
       </c>
@@ -4606,8 +4815,11 @@
       <c r="L62" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>188</v>
       </c>
@@ -4644,8 +4856,11 @@
       <c r="L63" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>190</v>
       </c>
@@ -4682,8 +4897,11 @@
       <c r="L64" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>191</v>
       </c>
@@ -4720,8 +4938,11 @@
       <c r="L65" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>194</v>
       </c>
@@ -4758,8 +4979,11 @@
       <c r="L66" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>197</v>
       </c>
@@ -4796,8 +5020,11 @@
       <c r="L67" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>199</v>
       </c>
@@ -4834,8 +5061,11 @@
       <c r="L68" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>201</v>
       </c>
@@ -4872,8 +5102,11 @@
       <c r="L69" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>204</v>
       </c>
@@ -4910,8 +5143,11 @@
       <c r="L70" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>206</v>
       </c>
@@ -4948,8 +5184,11 @@
       <c r="L71" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>209</v>
       </c>
@@ -4986,8 +5225,11 @@
       <c r="L72" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>211</v>
       </c>
@@ -5024,8 +5266,11 @@
       <c r="L73" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>213</v>
       </c>
@@ -5062,8 +5307,11 @@
       <c r="L74" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>215</v>
       </c>
@@ -5100,8 +5348,11 @@
       <c r="L75" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>217</v>
       </c>
@@ -5138,8 +5389,11 @@
       <c r="L76" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>220</v>
       </c>
@@ -5176,8 +5430,11 @@
       <c r="L77" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>222</v>
       </c>
@@ -5214,8 +5471,11 @@
       <c r="L78" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>225</v>
       </c>
@@ -5252,8 +5512,11 @@
       <c r="L79" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>227</v>
       </c>
@@ -5290,8 +5553,11 @@
       <c r="L80" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>229</v>
       </c>
@@ -5328,8 +5594,11 @@
       <c r="L81" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>231</v>
       </c>
@@ -5366,8 +5635,11 @@
       <c r="L82" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>232</v>
       </c>
@@ -5404,8 +5676,11 @@
       <c r="L83" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>234</v>
       </c>
@@ -5442,8 +5717,11 @@
       <c r="L84" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>236</v>
       </c>
@@ -5480,8 +5758,11 @@
       <c r="L85" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>238</v>
       </c>
@@ -5518,8 +5799,11 @@
       <c r="L86" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>240</v>
       </c>
@@ -5556,8 +5840,11 @@
       <c r="L87" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>243</v>
       </c>
@@ -5594,8 +5881,11 @@
       <c r="L88" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>246</v>
       </c>
@@ -5632,8 +5922,11 @@
       <c r="L89" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>247</v>
       </c>
@@ -5670,8 +5963,11 @@
       <c r="L90" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>249</v>
       </c>
@@ -5708,8 +6004,11 @@
       <c r="L91" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>251</v>
       </c>
@@ -5746,8 +6045,11 @@
       <c r="L92" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>253</v>
       </c>
@@ -5784,8 +6086,11 @@
       <c r="L93" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>257</v>
       </c>
@@ -5822,8 +6127,11 @@
       <c r="L94" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>258</v>
       </c>
@@ -5860,8 +6168,11 @@
       <c r="L95" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>260</v>
       </c>
@@ -5898,8 +6209,11 @@
       <c r="L96" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>261</v>
       </c>
@@ -5936,8 +6250,11 @@
       <c r="L97" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>262</v>
       </c>
@@ -5974,8 +6291,11 @@
       <c r="L98" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>265</v>
       </c>
@@ -6012,8 +6332,11 @@
       <c r="L99" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>266</v>
       </c>
@@ -6050,8 +6373,11 @@
       <c r="L100" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>268</v>
       </c>
@@ -6088,8 +6414,11 @@
       <c r="L101" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>125</v>
       </c>
@@ -6126,8 +6455,11 @@
       <c r="L102" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>274</v>
       </c>
@@ -6164,8 +6496,11 @@
       <c r="L103" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>276</v>
       </c>
@@ -6202,8 +6537,11 @@
       <c r="L104" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>278</v>
       </c>
@@ -6240,8 +6578,11 @@
       <c r="L105" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>280</v>
       </c>
@@ -6278,8 +6619,11 @@
       <c r="L106" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>282</v>
       </c>
@@ -6316,8 +6660,11 @@
       <c r="L107" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>284</v>
       </c>
@@ -6354,8 +6701,11 @@
       <c r="L108" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>287</v>
       </c>
@@ -6392,8 +6742,11 @@
       <c r="L109" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>291</v>
       </c>
@@ -6430,8 +6783,11 @@
       <c r="L110" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>292</v>
       </c>
@@ -6468,8 +6824,11 @@
       <c r="L111" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>294</v>
       </c>
@@ -6506,8 +6865,11 @@
       <c r="L112" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>295</v>
       </c>
@@ -6544,8 +6906,11 @@
       <c r="L113" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>296</v>
       </c>
@@ -6582,8 +6947,11 @@
       <c r="L114" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>299</v>
       </c>
@@ -6620,8 +6988,11 @@
       <c r="L115" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>301</v>
       </c>
@@ -6658,8 +7029,11 @@
       <c r="L116" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>302</v>
       </c>
@@ -6696,8 +7070,11 @@
       <c r="L117" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>303</v>
       </c>
@@ -6734,8 +7111,11 @@
       <c r="L118" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>304</v>
       </c>
@@ -6772,8 +7152,11 @@
       <c r="L119" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>305</v>
       </c>
@@ -6810,8 +7193,11 @@
       <c r="L120" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>306</v>
       </c>
@@ -6848,8 +7234,11 @@
       <c r="L121" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>308</v>
       </c>
@@ -6886,8 +7275,11 @@
       <c r="L122" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>309</v>
       </c>
@@ -6924,8 +7316,11 @@
       <c r="L123" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>312</v>
       </c>
@@ -6962,8 +7357,11 @@
       <c r="L124" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>314</v>
       </c>
@@ -7000,8 +7398,11 @@
       <c r="L125" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>315</v>
       </c>
@@ -7038,8 +7439,11 @@
       <c r="L126" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>317</v>
       </c>
@@ -7076,8 +7480,11 @@
       <c r="L127" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>318</v>
       </c>
@@ -7114,8 +7521,11 @@
       <c r="L128" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>319</v>
       </c>
@@ -7152,8 +7562,11 @@
       <c r="L129" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>320</v>
       </c>
@@ -7190,8 +7603,11 @@
       <c r="L130" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>321</v>
       </c>
@@ -7228,8 +7644,11 @@
       <c r="L131" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>323</v>
       </c>
@@ -7266,8 +7685,11 @@
       <c r="L132" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>324</v>
       </c>
@@ -7304,8 +7726,11 @@
       <c r="L133" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>325</v>
       </c>
@@ -7342,8 +7767,11 @@
       <c r="L134" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>327</v>
       </c>
@@ -7380,8 +7808,11 @@
       <c r="L135" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>329</v>
       </c>
@@ -7418,8 +7849,11 @@
       <c r="L136" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>331</v>
       </c>
@@ -7456,8 +7890,11 @@
       <c r="L137" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>332</v>
       </c>
@@ -7494,8 +7931,11 @@
       <c r="L138" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>333</v>
       </c>
@@ -7532,8 +7972,11 @@
       <c r="L139" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>335</v>
       </c>
@@ -7570,8 +8013,11 @@
       <c r="L140" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>336</v>
       </c>
@@ -7608,8 +8054,11 @@
       <c r="L141" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>339</v>
       </c>
@@ -7646,8 +8095,11 @@
       <c r="L142" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M142" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>341</v>
       </c>
@@ -7684,8 +8136,11 @@
       <c r="L143" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>344</v>
       </c>
@@ -7722,8 +8177,11 @@
       <c r="L144" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M144" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>346</v>
       </c>
@@ -7760,8 +8218,11 @@
       <c r="L145" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M145" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>349</v>
       </c>
@@ -7798,8 +8259,11 @@
       <c r="L146" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M146" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>350</v>
       </c>
@@ -7836,8 +8300,11 @@
       <c r="L147" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M147" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>352</v>
       </c>
@@ -7874,8 +8341,11 @@
       <c r="L148" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M148" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>354</v>
       </c>
@@ -7912,8 +8382,11 @@
       <c r="L149" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M149" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>356</v>
       </c>
@@ -7950,8 +8423,11 @@
       <c r="L150" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M150" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>358</v>
       </c>
@@ -7988,8 +8464,11 @@
       <c r="L151" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M151" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>360</v>
       </c>
@@ -8026,8 +8505,11 @@
       <c r="L152" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M152" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>361</v>
       </c>
@@ -8064,8 +8546,11 @@
       <c r="L153" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M153" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>362</v>
       </c>
@@ -8102,8 +8587,11 @@
       <c r="L154" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M154" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>363</v>
       </c>
@@ -8140,8 +8628,11 @@
       <c r="L155" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M155" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>364</v>
       </c>
@@ -8178,8 +8669,11 @@
       <c r="L156" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M156" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>366</v>
       </c>
@@ -8216,8 +8710,11 @@
       <c r="L157" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M157" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>369</v>
       </c>
@@ -8254,8 +8751,11 @@
       <c r="L158" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M158" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>371</v>
       </c>
@@ -8292,8 +8792,11 @@
       <c r="L159" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M159" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>373</v>
       </c>
@@ -8330,8 +8833,11 @@
       <c r="L160" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M160" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>375</v>
       </c>
@@ -8368,8 +8874,11 @@
       <c r="L161" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M161" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>376</v>
       </c>
@@ -8406,8 +8915,11 @@
       <c r="L162" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M162" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>378</v>
       </c>
@@ -8444,8 +8956,11 @@
       <c r="L163" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M163" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>381</v>
       </c>
@@ -8482,8 +8997,11 @@
       <c r="L164" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M164" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>383</v>
       </c>
@@ -8520,8 +9038,11 @@
       <c r="L165" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M165" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>385</v>
       </c>
@@ -8558,8 +9079,11 @@
       <c r="L166" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M166" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>387</v>
       </c>
@@ -8596,8 +9120,11 @@
       <c r="L167" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M167" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>389</v>
       </c>
@@ -8634,8 +9161,11 @@
       <c r="L168" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M168" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>390</v>
       </c>
@@ -8672,8 +9202,11 @@
       <c r="L169" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M169" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>391</v>
       </c>
@@ -8710,8 +9243,11 @@
       <c r="L170" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M170" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>393</v>
       </c>
@@ -8748,8 +9284,11 @@
       <c r="L171" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M171" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>394</v>
       </c>
@@ -8786,8 +9325,11 @@
       <c r="L172" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M172" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>396</v>
       </c>
@@ -8824,8 +9366,11 @@
       <c r="L173" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M173" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>398</v>
       </c>
@@ -8862,8 +9407,11 @@
       <c r="L174" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M174" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>400</v>
       </c>
@@ -8900,8 +9448,11 @@
       <c r="L175" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M175" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>402</v>
       </c>
@@ -8938,8 +9489,11 @@
       <c r="L176" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M176" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>403</v>
       </c>
@@ -8976,8 +9530,11 @@
       <c r="L177" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M177" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>404</v>
       </c>
@@ -9014,8 +9571,11 @@
       <c r="L178" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M178" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>405</v>
       </c>
@@ -9052,8 +9612,11 @@
       <c r="L179" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M179" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>406</v>
       </c>
@@ -9090,8 +9653,11 @@
       <c r="L180" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M180" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>407</v>
       </c>
@@ -9128,8 +9694,11 @@
       <c r="L181" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M181" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>408</v>
       </c>
@@ -9166,8 +9735,11 @@
       <c r="L182" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M182" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>409</v>
       </c>
@@ -9204,8 +9776,11 @@
       <c r="L183" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M183" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>411</v>
       </c>
@@ -9242,8 +9817,11 @@
       <c r="L184" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M184" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>413</v>
       </c>
@@ -9280,8 +9858,11 @@
       <c r="L185" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M185" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>414</v>
       </c>
@@ -9318,8 +9899,11 @@
       <c r="L186" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M186" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>416</v>
       </c>
@@ -9356,8 +9940,11 @@
       <c r="L187" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M187" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>419</v>
       </c>
@@ -9394,8 +9981,11 @@
       <c r="L188" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M188" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>420</v>
       </c>
@@ -9432,8 +10022,11 @@
       <c r="L189" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M189" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>423</v>
       </c>
@@ -9470,8 +10063,11 @@
       <c r="L190" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M190" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>425</v>
       </c>
@@ -9508,8 +10104,11 @@
       <c r="L191" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M191" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>426</v>
       </c>
@@ -9546,8 +10145,11 @@
       <c r="L192" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M192" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>428</v>
       </c>
@@ -9584,8 +10186,11 @@
       <c r="L193" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M193" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>429</v>
       </c>
@@ -9622,8 +10227,11 @@
       <c r="L194" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M194" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>430</v>
       </c>
@@ -9660,8 +10268,11 @@
       <c r="L195" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M195" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>431</v>
       </c>
@@ -9698,8 +10309,11 @@
       <c r="L196" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M196" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>432</v>
       </c>
@@ -9736,8 +10350,11 @@
       <c r="L197" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M197" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>434</v>
       </c>
@@ -9774,8 +10391,11 @@
       <c r="L198" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M198" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>436</v>
       </c>
@@ -9812,8 +10432,11 @@
       <c r="L199" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M199" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>438</v>
       </c>
@@ -9850,8 +10473,11 @@
       <c r="L200" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M200" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>441</v>
       </c>
@@ -9888,8 +10514,11 @@
       <c r="L201" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M201" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>442</v>
       </c>
@@ -9926,8 +10555,11 @@
       <c r="L202" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M202" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>444</v>
       </c>
@@ -9964,8 +10596,11 @@
       <c r="L203" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M203" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>445</v>
       </c>
@@ -10002,8 +10637,11 @@
       <c r="L204" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M204" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>446</v>
       </c>
@@ -10040,8 +10678,11 @@
       <c r="L205" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M205" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>447</v>
       </c>
@@ -10078,8 +10719,11 @@
       <c r="L206" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M206" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>448</v>
       </c>
@@ -10116,8 +10760,11 @@
       <c r="L207" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M207" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>450</v>
       </c>
@@ -10154,8 +10801,11 @@
       <c r="L208" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M208" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>451</v>
       </c>
@@ -10192,8 +10842,11 @@
       <c r="L209" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M209" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>452</v>
       </c>
@@ -10230,8 +10883,11 @@
       <c r="L210" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M210" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>453</v>
       </c>
@@ -10268,8 +10924,11 @@
       <c r="L211" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M211" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>454</v>
       </c>
@@ -10305,6 +10964,214 @@
       </c>
       <c r="L212" t="s">
         <v>17</v>
+      </c>
+      <c r="M212" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>456</v>
+      </c>
+      <c r="B213" t="s">
+        <v>13</v>
+      </c>
+      <c r="C213" t="s">
+        <v>35</v>
+      </c>
+      <c r="D213" t="s">
+        <v>133</v>
+      </c>
+      <c r="E213" s="1">
+        <v>44637</v>
+      </c>
+      <c r="F213" t="s">
+        <v>137</v>
+      </c>
+      <c r="G213">
+        <v>164</v>
+      </c>
+      <c r="H213" t="s">
+        <v>103</v>
+      </c>
+      <c r="I213" t="s">
+        <v>22</v>
+      </c>
+      <c r="J213" t="s">
+        <v>121</v>
+      </c>
+      <c r="K213">
+        <v>5</v>
+      </c>
+      <c r="L213" t="s">
+        <v>17</v>
+      </c>
+      <c r="M213" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>457</v>
+      </c>
+      <c r="B214" t="s">
+        <v>13</v>
+      </c>
+      <c r="C214" t="s">
+        <v>36</v>
+      </c>
+      <c r="D214" t="s">
+        <v>62</v>
+      </c>
+      <c r="E214" s="1">
+        <v>44734</v>
+      </c>
+      <c r="F214" t="s">
+        <v>77</v>
+      </c>
+      <c r="G214">
+        <v>158</v>
+      </c>
+      <c r="H214" t="s">
+        <v>458</v>
+      </c>
+      <c r="I214" t="s">
+        <v>43</v>
+      </c>
+      <c r="J214" t="s">
+        <v>48</v>
+      </c>
+      <c r="K214">
+        <v>5</v>
+      </c>
+      <c r="L214" t="s">
+        <v>17</v>
+      </c>
+      <c r="M214" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>459</v>
+      </c>
+      <c r="B215" t="s">
+        <v>13</v>
+      </c>
+      <c r="C215" t="s">
+        <v>36</v>
+      </c>
+      <c r="D215" t="s">
+        <v>168</v>
+      </c>
+      <c r="E215" s="1">
+        <v>44627</v>
+      </c>
+      <c r="F215" t="s">
+        <v>36</v>
+      </c>
+      <c r="G215">
+        <v>166</v>
+      </c>
+      <c r="H215" t="s">
+        <v>460</v>
+      </c>
+      <c r="I215" t="s">
+        <v>86</v>
+      </c>
+      <c r="J215" t="s">
+        <v>210</v>
+      </c>
+      <c r="K215">
+        <v>6</v>
+      </c>
+      <c r="L215" t="s">
+        <v>17</v>
+      </c>
+      <c r="M215" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>461</v>
+      </c>
+      <c r="B216" t="s">
+        <v>13</v>
+      </c>
+      <c r="C216" t="s">
+        <v>35</v>
+      </c>
+      <c r="D216" t="s">
+        <v>151</v>
+      </c>
+      <c r="E216" s="1">
+        <v>44749</v>
+      </c>
+      <c r="F216" t="s">
+        <v>254</v>
+      </c>
+      <c r="G216">
+        <v>168</v>
+      </c>
+      <c r="H216" t="s">
+        <v>241</v>
+      </c>
+      <c r="I216" t="s">
+        <v>39</v>
+      </c>
+      <c r="J216" t="s">
+        <v>273</v>
+      </c>
+      <c r="K216">
+        <v>6</v>
+      </c>
+      <c r="L216" t="s">
+        <v>256</v>
+      </c>
+      <c r="M216" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>462</v>
+      </c>
+      <c r="B217" t="s">
+        <v>13</v>
+      </c>
+      <c r="C217" t="s">
+        <v>25</v>
+      </c>
+      <c r="D217" t="s">
+        <v>51</v>
+      </c>
+      <c r="E217" s="1">
+        <v>44674</v>
+      </c>
+      <c r="F217" t="s">
+        <v>52</v>
+      </c>
+      <c r="G217">
+        <v>171</v>
+      </c>
+      <c r="H217" t="s">
+        <v>103</v>
+      </c>
+      <c r="I217" t="s">
+        <v>22</v>
+      </c>
+      <c r="J217" t="s">
+        <v>23</v>
+      </c>
+      <c r="K217">
+        <v>6</v>
+      </c>
+      <c r="L217" t="s">
+        <v>185</v>
+      </c>
+      <c r="M217" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update statistic, add headhunt simulator
</commit_message>
<xml_diff>
--- a/WriteData/operators.xlsx
+++ b/WriteData/operators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Web\ArknightsTools\WriteData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD429EF-B5F9-44CF-BDF8-D54DF8DD91CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140644EF-0C15-427B-9145-CB5457B607E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1984" uniqueCount="464">
   <si>
     <t>codeName</t>
   </si>
@@ -1409,6 +1409,9 @@
   </si>
   <si>
     <t>Nine-Colored Deer</t>
+  </si>
+  <si>
+    <t>Shalem</t>
   </si>
 </sst>
 </file>
@@ -2253,11 +2256,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M218"/>
+  <dimension ref="A1:M219"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I220" sqref="I220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7106,7 +7109,7 @@
         <v>118</v>
       </c>
       <c r="K118">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L118" t="s">
         <v>17</v>
@@ -11212,6 +11215,47 @@
         <v>17</v>
       </c>
       <c r="M218" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>463</v>
+      </c>
+      <c r="B219" t="s">
+        <v>20</v>
+      </c>
+      <c r="C219" t="s">
+        <v>113</v>
+      </c>
+      <c r="D219" t="s">
+        <v>61</v>
+      </c>
+      <c r="E219" s="1">
+        <v>44904</v>
+      </c>
+      <c r="F219" t="s">
+        <v>366</v>
+      </c>
+      <c r="G219">
+        <v>179</v>
+      </c>
+      <c r="H219" t="s">
+        <v>240</v>
+      </c>
+      <c r="I219" t="s">
+        <v>31</v>
+      </c>
+      <c r="J219" t="s">
+        <v>278</v>
+      </c>
+      <c r="K219">
+        <v>5</v>
+      </c>
+      <c r="L219" t="s">
+        <v>17</v>
+      </c>
+      <c r="M219" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>